<commit_message>
FAQs, fixed broken UAR link. Some additional info on admission
</commit_message>
<xml_diff>
--- a/blog/content/KurseMscECMX.xlsx
+++ b/blog/content/KurseMscECMX.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martin/WebEcon/blog/content/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7FB739-196D-AB46-BCBC-64A60AE2B8BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679AB3FB-4084-8644-844E-578B92092114}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2352,8 +2352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A3:AML124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C74" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="L78" sqref="L78"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
@@ -2652,7 +2652,7 @@
         <v>69</v>
       </c>
       <c r="Q7" s="17">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="R7" s="17" t="s">
         <v>371</v>
@@ -4486,10 +4486,10 @@
         <v>150</v>
       </c>
       <c r="Q39" s="17">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="R39" s="17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="S39" s="17" t="s">
         <v>399</v>

</xml_diff>